<commit_message>
add car functions api
</commit_message>
<xml_diff>
--- a/public/excel/MapUsers.xlsx
+++ b/public/excel/MapUsers.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\waritexGoogle\public\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1D59F450-35A9-46E3-B5C5-EA5CC3DD5769}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9A1E67E-F982-4DFB-8D5D-9DA71D43FC39}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" xr2:uid="{6AF17357-B30C-47A3-8A67-5EF7ABC6544F}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t>username</t>
   </si>
@@ -87,6 +87,33 @@
   </si>
   <si>
     <t>IRQ009</t>
+  </si>
+  <si>
+    <t>صالح الماضي</t>
+  </si>
+  <si>
+    <t>IRQ200</t>
+  </si>
+  <si>
+    <t>carcode</t>
+  </si>
+  <si>
+    <t>waritex11123</t>
+  </si>
+  <si>
+    <t>waritex107</t>
+  </si>
+  <si>
+    <t>waritex3</t>
+  </si>
+  <si>
+    <t>waritex6</t>
+  </si>
+  <si>
+    <t>waritex7</t>
+  </si>
+  <si>
+    <t>waritex8</t>
   </si>
 </sst>
 </file>
@@ -131,7 +158,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="8">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -167,14 +197,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{47ADD053-1F91-4DE5-B9C0-2661E75A3233}" name="Table1" displayName="Table1" ref="A1:E8" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
-  <autoFilter ref="A1:E8" xr:uid="{48B50E91-FA5E-475A-B9DA-955694920C2A}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{08296B01-347D-4DE6-926B-8F72C06C0A96}" name="username" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{EBB031FC-0963-4BBB-85B4-F9C935962107}" name="code" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{B6356E5C-112A-4D08-B0D8-9D93851D14FD}" name="name" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{A23255C8-A2F0-445D-87EE-97C1FA12C32A}" name="supervisor" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{B41DB399-1F54-46A5-B271-09717F75C24D}" name="buid" dataDxfId="2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{47ADD053-1F91-4DE5-B9C0-2661E75A3233}" name="Table1" displayName="Table1" ref="A1:F9" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F9" xr:uid="{48B50E91-FA5E-475A-B9DA-955694920C2A}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{08296B01-347D-4DE6-926B-8F72C06C0A96}" name="username" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{EBB031FC-0963-4BBB-85B4-F9C935962107}" name="code" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{B6356E5C-112A-4D08-B0D8-9D93851D14FD}" name="name" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{A23255C8-A2F0-445D-87EE-97C1FA12C32A}" name="supervisor" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{B41DB399-1F54-46A5-B271-09717F75C24D}" name="buid" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{F1EAB156-BC32-43FE-88BB-E3A6983FF61C}" name="carcode" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -477,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F93B4992-B3D2-4D71-A6A3-A97206BBEA85}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,9 +521,10 @@
     <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -508,8 +540,11 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -525,8 +560,11 @@
       <c r="E2" s="1">
         <v>105</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -542,8 +580,11 @@
       <c r="E3" s="1">
         <v>105</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -559,8 +600,11 @@
       <c r="E4" s="1">
         <v>105</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -576,8 +620,11 @@
       <c r="E5" s="1">
         <v>105</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -593,8 +640,11 @@
       <c r="E6" s="1">
         <v>105</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
@@ -610,8 +660,11 @@
       <c r="E7" s="1">
         <v>105</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -627,6 +680,25 @@
       <c r="E8" s="1">
         <v>105</v>
       </c>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1">
+        <v>105</v>
+      </c>
+      <c r="F9" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>